<commit_message>
Add newest status of MagicItems.xlsx
</commit_message>
<xml_diff>
--- a/resources/db/MagicItems.xlsx
+++ b/resources/db/MagicItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84A70E9-3EAF-47E7-A6B5-654C0A4838B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74871AB4-4E2F-4C0A-BAF0-2135759060B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Unique items" sheetId="1" r:id="rId1"/>
     <sheet name="Unique items 2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Unique items 2'!$A$1:$J$184</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="373">
   <si>
     <t>id</t>
   </si>
@@ -1148,6 +1151,12 @@
   </si>
   <si>
     <t>Loki Weissbart</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -5848,11 +5857,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725527C8-E57F-482B-B66A-C63CCC7FE491}">
-  <dimension ref="A1:I184"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5864,7 +5874,7 @@
     <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -5892,8 +5902,11 @@
       <c r="I1" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -5922,7 +5935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5951,7 +5964,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5980,7 +5993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -6009,7 +6022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -6038,7 +6051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -6067,7 +6080,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -6096,7 +6109,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6125,7 +6138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6154,7 +6167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -6183,7 +6196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -6212,7 +6225,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -6241,7 +6254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -6270,7 +6283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -6299,7 +6312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -6328,7 +6341,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -6357,7 +6370,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -6385,8 +6398,11 @@
       <c r="I18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -6415,7 +6431,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -6444,7 +6460,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -6473,7 +6489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -6502,7 +6518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -6531,7 +6547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -6560,7 +6576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -6589,7 +6605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -6618,7 +6634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -6647,7 +6663,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -6676,7 +6692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -6705,7 +6721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -6734,7 +6750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -6763,7 +6779,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -6792,7 +6808,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -6821,7 +6837,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -6850,7 +6866,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -6879,7 +6895,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -6908,7 +6924,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -6937,7 +6953,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -6966,7 +6982,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -6995,7 +7011,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -7082,7 +7098,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -7111,7 +7127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -7140,7 +7156,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -7401,7 +7417,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -7430,7 +7446,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -7459,7 +7475,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -7488,7 +7504,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -7517,7 +7533,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -7546,7 +7562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -7575,7 +7591,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -7604,7 +7620,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -7633,7 +7649,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -7662,7 +7678,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>42</v>
       </c>
@@ -7691,7 +7707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -7720,7 +7736,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -7749,7 +7765,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -7778,7 +7794,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>42</v>
       </c>
@@ -7807,7 +7823,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>42</v>
       </c>
@@ -7836,7 +7852,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>42</v>
       </c>
@@ -7865,7 +7881,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -7894,7 +7910,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -7923,7 +7939,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -7952,7 +7968,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -7981,7 +7997,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -8010,7 +8026,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -8039,7 +8055,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -8068,7 +8084,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -8097,7 +8113,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>42</v>
       </c>
@@ -8126,7 +8142,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>42</v>
       </c>
@@ -8503,7 +8519,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -8532,7 +8548,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -8561,7 +8577,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -8590,7 +8606,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>106</v>
       </c>
@@ -8619,7 +8635,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>106</v>
       </c>
@@ -8648,7 +8664,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -8677,7 +8693,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -8706,7 +8722,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -8735,7 +8751,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -8764,7 +8780,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>106</v>
       </c>
@@ -8793,7 +8809,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -8822,7 +8838,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -8851,7 +8867,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -8880,7 +8896,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -9112,7 +9128,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>106</v>
       </c>
@@ -9141,7 +9157,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>106</v>
       </c>
@@ -9170,7 +9186,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>106</v>
       </c>
@@ -9199,7 +9215,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>106</v>
       </c>
@@ -9228,7 +9244,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>106</v>
       </c>
@@ -9257,7 +9273,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>106</v>
       </c>
@@ -9286,7 +9302,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>106</v>
       </c>
@@ -9315,7 +9331,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>106</v>
       </c>
@@ -9344,7 +9360,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>106</v>
       </c>
@@ -9373,7 +9389,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>106</v>
       </c>
@@ -9402,7 +9418,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>106</v>
       </c>
@@ -9431,7 +9447,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>106</v>
       </c>
@@ -9808,7 +9824,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>106</v>
       </c>
@@ -9837,7 +9853,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>106</v>
       </c>
@@ -9866,7 +9882,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>106</v>
       </c>
@@ -9895,7 +9911,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>106</v>
       </c>
@@ -9924,7 +9940,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>106</v>
       </c>
@@ -9953,7 +9969,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>106</v>
       </c>
@@ -9982,7 +9998,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>106</v>
       </c>
@@ -10011,7 +10027,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>106</v>
       </c>
@@ -10040,7 +10056,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>106</v>
       </c>
@@ -10069,7 +10085,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>106</v>
       </c>
@@ -10098,7 +10114,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>106</v>
       </c>
@@ -10127,7 +10143,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>106</v>
       </c>
@@ -10156,7 +10172,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>106</v>
       </c>
@@ -10185,7 +10201,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>106</v>
       </c>
@@ -10214,7 +10230,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>106</v>
       </c>
@@ -10243,7 +10259,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>106</v>
       </c>
@@ -10272,7 +10288,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>106</v>
       </c>
@@ -10301,7 +10317,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>106</v>
       </c>
@@ -10330,7 +10346,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>106</v>
       </c>
@@ -10359,7 +10375,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>106</v>
       </c>
@@ -10388,7 +10404,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>106</v>
       </c>
@@ -10417,7 +10433,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>106</v>
       </c>
@@ -10446,7 +10462,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>106</v>
       </c>
@@ -10475,7 +10491,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>106</v>
       </c>
@@ -10504,7 +10520,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>106</v>
       </c>
@@ -10533,7 +10549,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>106</v>
       </c>
@@ -10562,7 +10578,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>106</v>
       </c>
@@ -10591,7 +10607,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>106</v>
       </c>
@@ -10620,7 +10636,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>106</v>
       </c>
@@ -10649,7 +10665,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>106</v>
       </c>
@@ -10881,7 +10897,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>188</v>
       </c>
@@ -10939,7 +10955,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>188</v>
       </c>
@@ -10968,7 +10984,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>188</v>
       </c>
@@ -10997,7 +11013,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>188</v>
       </c>
@@ -11026,7 +11042,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>194</v>
       </c>
@@ -11055,7 +11071,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -11084,7 +11100,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>194</v>
       </c>
@@ -11113,7 +11129,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>194</v>
       </c>
@@ -11142,7 +11158,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>199</v>
       </c>
@@ -11201,6 +11217,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J184" xr:uid="{725527C8-E57F-482B-B66A-C63CCC7FE491}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Dunkelelfen"/>
+        <filter val="Hochelfen"/>
+        <filter val="Zwerge"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WiP: Check unique item
</commit_message>
<xml_diff>
--- a/resources/db/MagicItems.xlsx
+++ b/resources/db/MagicItems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74871AB4-4E2F-4C0A-BAF0-2135759060B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D12089-26E4-4471-B36D-1C4B3BC2C323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
+    <workbookView xWindow="3495" yWindow="330" windowWidth="7725" windowHeight="15150" activeTab="1" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
   </bookViews>
   <sheets>
     <sheet name="Unique items" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="374">
   <si>
     <t>id</t>
   </si>
@@ -1157,6 +1157,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1219,9 +1222,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1259,7 +1262,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1365,7 +1368,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1507,7 +1510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5860,17 +5863,17 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6079,8 +6082,11 @@
       <c r="I7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -6108,8 +6114,11 @@
       <c r="I8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6137,8 +6146,11 @@
       <c r="I9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6166,8 +6178,11 @@
       <c r="I10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -6195,8 +6210,11 @@
       <c r="I11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -6224,8 +6242,11 @@
       <c r="I12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -6253,8 +6274,11 @@
       <c r="I13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -6281,6 +6305,9 @@
       </c>
       <c r="I14" t="s">
         <v>17</v>
+      </c>
+      <c r="J14" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -6518,7 +6545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -6546,8 +6573,11 @@
       <c r="I23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -6575,8 +6605,11 @@
       <c r="I24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -6604,8 +6637,11 @@
       <c r="I25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -6633,8 +6669,11 @@
       <c r="I26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -6662,8 +6701,11 @@
       <c r="I27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -6691,8 +6733,11 @@
       <c r="I28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -6720,6 +6765,9 @@
       <c r="I29" t="s">
         <v>36</v>
       </c>
+      <c r="J29" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -6808,7 +6856,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -6837,7 +6885,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -6866,7 +6914,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -6895,7 +6943,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -6924,7 +6972,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -6953,7 +7001,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -6982,7 +7030,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -7011,7 +7059,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -7040,7 +7088,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -7068,8 +7116,11 @@
       <c r="I41" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -7097,8 +7148,11 @@
       <c r="I42" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -7127,7 +7181,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -7156,7 +7210,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -7185,7 +7239,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -7213,8 +7267,11 @@
       <c r="I46" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -7242,8 +7299,11 @@
       <c r="I47" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -7271,8 +7331,11 @@
       <c r="I48" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -7300,8 +7363,11 @@
       <c r="I49" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -7329,8 +7395,11 @@
       <c r="I50" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -7359,7 +7428,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -7388,7 +7457,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -7417,7 +7486,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -7446,7 +7515,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -7475,7 +7544,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -7504,7 +7573,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -7533,7 +7602,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -7562,7 +7631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -7591,7 +7660,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -7620,7 +7689,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -7649,7 +7718,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -7678,7 +7747,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>42</v>
       </c>
@@ -7707,7 +7776,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -8171,7 +8240,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -8200,7 +8269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -8229,7 +8298,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>42</v>
       </c>
@@ -8258,7 +8327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -8287,7 +8356,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -8316,7 +8385,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -8345,7 +8414,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -8374,7 +8443,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>42</v>
       </c>
@@ -8403,7 +8472,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>42</v>
       </c>
@@ -8432,7 +8501,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>42</v>
       </c>
@@ -8461,7 +8530,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>42</v>
       </c>
@@ -8490,7 +8559,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -8664,7 +8733,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -8693,7 +8762,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -8722,7 +8791,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -8751,7 +8820,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -8780,7 +8849,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>106</v>
       </c>
@@ -8809,7 +8878,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -8838,7 +8907,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -8867,7 +8936,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -8896,7 +8965,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -8925,7 +8994,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -8953,8 +9022,11 @@
       <c r="I106" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -8982,8 +9054,11 @@
       <c r="I107" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -9012,7 +9087,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>106</v>
       </c>
@@ -9041,7 +9116,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>106</v>
       </c>
@@ -9070,7 +9145,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>106</v>
       </c>
@@ -9099,7 +9174,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>106</v>
       </c>
@@ -9476,7 +9551,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>106</v>
       </c>
@@ -9505,7 +9580,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>106</v>
       </c>
@@ -9534,7 +9609,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>106</v>
       </c>
@@ -9563,7 +9638,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>106</v>
       </c>
@@ -9592,7 +9667,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>106</v>
       </c>
@@ -9621,7 +9696,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>106</v>
       </c>
@@ -9650,7 +9725,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>106</v>
       </c>
@@ -9678,8 +9753,11 @@
       <c r="I131" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>106</v>
       </c>
@@ -9707,8 +9785,11 @@
       <c r="I132" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>106</v>
       </c>
@@ -9736,8 +9817,11 @@
       <c r="I133" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>106</v>
       </c>
@@ -9765,8 +9849,11 @@
       <c r="I134" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>106</v>
       </c>
@@ -9795,7 +9882,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>106</v>
       </c>
@@ -9824,7 +9911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>106</v>
       </c>
@@ -9853,7 +9940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>106</v>
       </c>
@@ -9882,7 +9969,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>106</v>
       </c>
@@ -9911,7 +9998,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>106</v>
       </c>
@@ -9940,7 +10027,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>106</v>
       </c>
@@ -9969,7 +10056,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>106</v>
       </c>
@@ -9998,7 +10085,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>106</v>
       </c>
@@ -10027,7 +10114,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>106</v>
       </c>
@@ -10694,7 +10781,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>106</v>
       </c>
@@ -10723,7 +10810,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>106</v>
       </c>
@@ -10752,7 +10839,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>106</v>
       </c>
@@ -10781,7 +10868,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>106</v>
       </c>
@@ -10810,7 +10897,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>106</v>
       </c>
@@ -10839,7 +10926,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>106</v>
       </c>
@@ -10868,7 +10955,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>106</v>
       </c>
@@ -10926,7 +11013,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>188</v>
       </c>
@@ -11187,7 +11274,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>199</v>
       </c>
@@ -11221,8 +11308,6 @@
     <filterColumn colId="1">
       <filters>
         <filter val="Dunkelelfen"/>
-        <filter val="Hochelfen"/>
-        <filter val="Zwerge"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Started updating description of magic items
</commit_message>
<xml_diff>
--- a/resources/db/MagicItems.xlsx
+++ b/resources/db/MagicItems.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC02797-B4C6-4270-BCE6-856B51925157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00335357-5A7A-4929-B061-F66EF2AE2C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
   </bookViews>
   <sheets>
     <sheet name="Unique items" sheetId="1" r:id="rId1"/>
     <sheet name="Unique items 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Magic Items" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Unique items 2'!$A$1:$J$182</definedName>
@@ -33,12 +34,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="426">
   <si>
     <t>id</t>
   </si>
@@ -1160,6 +1164,162 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>RW von 2+, zweiter unmodifizierter RW von 4+.</t>
+  </si>
+  <si>
+    <t>Skaldors Rüstung</t>
+  </si>
+  <si>
+    <t>+2 auf Attacken</t>
+  </si>
+  <si>
+    <t>Schadenswurf ist immer 2+. Nur magische Rüstungen mit -3 auf RW. Jede Verletztung kostet W3 LP. Drachen und Dämonen verlieren W6 LP.</t>
+  </si>
+  <si>
+    <t>Kampfgeschick 10.</t>
+  </si>
+  <si>
+    <t>Gesegnetes Schwert</t>
+  </si>
+  <si>
+    <t>Schaden bei 2+, W3 LP, kein RW o. RW:-3. Drachen u. Dämonen W6 LP.</t>
+  </si>
+  <si>
+    <t>Gorteks Axt</t>
+  </si>
+  <si>
+    <t>Schaden bei 2+, W3 LP, kein RW o. RW:-3. W6 LP gegen Oger u. Trolle.</t>
+  </si>
+  <si>
+    <t>Grimnirs Axt</t>
+  </si>
+  <si>
+    <t>Verdoppelt Attacken in der ersten Kampfrunde. Nur für Waldgoblins.</t>
+  </si>
+  <si>
+    <t>Spinnenbanner</t>
+  </si>
+  <si>
+    <t>-1 auf Beschuß, Nachtgoblins attackieren immer zuerst</t>
+  </si>
+  <si>
+    <t>Das Halbmondbanner</t>
+  </si>
+  <si>
+    <t>Magie Bann bei 4+. Zauberer in Base-to-Base-Kontakt platzt der Kopf.</t>
+  </si>
+  <si>
+    <t>Morksbanner</t>
+  </si>
+  <si>
+    <t>Jeden verpatzten Stänkerei-Test wiederholen.</t>
+  </si>
+  <si>
+    <t>Das Sonnenfratzenbanner</t>
+  </si>
+  <si>
+    <t>Einheit erhält +1 auf Stärke in der ersten Kampfrunde.</t>
+  </si>
+  <si>
+    <t>Gorks Banner</t>
+  </si>
+  <si>
+    <t>Verursacht 2 Schadenspunkte, kein Rettungswurf.</t>
+  </si>
+  <si>
+    <t>Groms Axt</t>
+  </si>
+  <si>
+    <t>Träger attackiert immer zuerst. +1 auf KG, S und W, kein RW oder mit -3.</t>
+  </si>
+  <si>
+    <t>Morgors Axt</t>
+  </si>
+  <si>
+    <t>+1 auf Stärke. Pro Mob ein Blitz mit Reichweite: 24", Stärke: 4, RW: keiner.</t>
+  </si>
+  <si>
+    <t>Skarsniks Prodder</t>
+  </si>
+  <si>
+    <t>Erster Verpatzter Stänkereitest kann ignoriert werden. Nur für Orks und Wildorks</t>
+  </si>
+  <si>
+    <t>Borks Schwert</t>
+  </si>
+  <si>
+    <t>Trefferwurf darf einmal wiederholt werden.</t>
+  </si>
+  <si>
+    <t>Schwert der Gerechtigkeit</t>
+  </si>
+  <si>
+    <t>Kein Rettungswurf erlaubt. Untote verlieren 2 Lebenspunkte.</t>
+  </si>
+  <si>
+    <t>Runenklinge</t>
+  </si>
+  <si>
+    <t>Jeder Treffer verletzt automatisch. RW nur für magische Rüstungen.</t>
+  </si>
+  <si>
+    <t>Sigmars Hammer</t>
+  </si>
+  <si>
+    <t>Bei eigenem RW, erleidet der Gegner einen Treffer der Stärke 4.</t>
+  </si>
+  <si>
+    <t>Silbura Schild</t>
+  </si>
+  <si>
+    <t>-1 auf Stärke des Gegner, wenn er keine magische Waffe trägt.</t>
+  </si>
+  <si>
+    <t>Schattenrüstung</t>
+  </si>
+  <si>
+    <t>+2 Stärke beim Angriff. Trifft automatisch. Spezialattacke</t>
+  </si>
+  <si>
+    <t>Drachenklingenlanze</t>
+  </si>
+  <si>
+    <t>+3 auf Stärke für einen Spielzug</t>
+  </si>
+  <si>
+    <t>Stärkungstrank</t>
+  </si>
+  <si>
+    <t>Ignoriert die Auswirkung von Blödheit. Nur für Echsenreiter.</t>
+  </si>
+  <si>
+    <t>Blutbanner</t>
+  </si>
+  <si>
+    <t>Opfer geköpft bei Schadenswurf von 6. Nur magische Rüstungen.</t>
+  </si>
+  <si>
+    <t>Axt des Henkers</t>
+  </si>
+  <si>
+    <t>Jede Verletztung kostet einen Punkt von KG und BF des Opfers.</t>
+  </si>
+  <si>
+    <t>Dunkles Schwert</t>
+  </si>
+  <si>
+    <t>Jede Treffer raubt bei 4+ einen magische Gegenstand oder Zauberspruch.</t>
+  </si>
+  <si>
+    <t>Zerstörer</t>
+  </si>
+  <si>
+    <t>Jede Verletzung kostet zusätzlich 1 Stärkepunkt.</t>
+  </si>
+  <si>
+    <t>Bluttrinker</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1185,6 +1345,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1201,9 +1367,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1222,9 +1389,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1262,7 +1429,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1368,7 +1535,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1510,7 +1677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5862,7 +6029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725527C8-E57F-482B-B66A-C63CCC7FE491}">
   <dimension ref="A1:J182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
@@ -11353,4 +11520,2406 @@
   <autoFilter ref="A1:J182" xr:uid="{725527C8-E57F-482B-B66A-C63CCC7FE491}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1508439D-2206-4762-B104-9E5E275BF891}">
+  <dimension ref="A1:H99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5655</v>
+      </c>
+      <c r="B2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5656</v>
+      </c>
+      <c r="B3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>422</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5665</v>
+      </c>
+      <c r="B4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5716</v>
+      </c>
+      <c r="B5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C5">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>378</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5896</v>
+      </c>
+      <c r="B6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>418</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5912</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5840</v>
+      </c>
+      <c r="B9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5937</v>
+      </c>
+      <c r="B10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>414</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5961</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5980</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6009</v>
+      </c>
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6036</v>
+      </c>
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6065</v>
+      </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5717</v>
+      </c>
+      <c r="B16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C16">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>378</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5733</v>
+      </c>
+      <c r="B17" t="s">
+        <v>413</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>412</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5869</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18">
+        <v>65</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5899</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5904</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5925</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5932</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22">
+        <v>125</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5940</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23">
+        <v>60</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6056</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5908</v>
+      </c>
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5793</v>
+      </c>
+      <c r="B26" t="s">
+        <v>411</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>410</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5959</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5979</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5998</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>6005</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6017</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>45</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5776</v>
+      </c>
+      <c r="B32" t="s">
+        <v>409</v>
+      </c>
+      <c r="C32">
+        <v>25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>408</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5842</v>
+      </c>
+      <c r="B33" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>201</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6076</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5939</v>
+      </c>
+      <c r="B35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35">
+        <v>35</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5989</v>
+      </c>
+      <c r="B36" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5995</v>
+      </c>
+      <c r="B37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37">
+        <v>50</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6007</v>
+      </c>
+      <c r="B38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>6028</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>6030</v>
+      </c>
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40">
+        <v>15</v>
+      </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6041</v>
+      </c>
+      <c r="B41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41">
+        <v>125</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6053</v>
+      </c>
+      <c r="B42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42">
+        <v>15</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6055</v>
+      </c>
+      <c r="B43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43">
+        <v>25</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6058</v>
+      </c>
+      <c r="B44" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44">
+        <v>85</v>
+      </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>6063</v>
+      </c>
+      <c r="B45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45">
+        <v>25</v>
+      </c>
+      <c r="E45">
+        <v>7</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6071</v>
+      </c>
+      <c r="B46" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46">
+        <v>55</v>
+      </c>
+      <c r="E46">
+        <v>7</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>5642</v>
+      </c>
+      <c r="B47" t="s">
+        <v>407</v>
+      </c>
+      <c r="C47">
+        <v>100</v>
+      </c>
+      <c r="D47" t="s">
+        <v>406</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5659</v>
+      </c>
+      <c r="B48" t="s">
+        <v>405</v>
+      </c>
+      <c r="C48">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>404</v>
+      </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>5692</v>
+      </c>
+      <c r="B49" t="s">
+        <v>403</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>402</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>5718</v>
+      </c>
+      <c r="B50" t="s">
+        <v>379</v>
+      </c>
+      <c r="C50">
+        <v>75</v>
+      </c>
+      <c r="D50" t="s">
+        <v>378</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5890</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51">
+        <v>100</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5936</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52">
+        <v>80</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5952</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53">
+        <v>75</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>5971</v>
+      </c>
+      <c r="B54" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54">
+        <v>40</v>
+      </c>
+      <c r="E54">
+        <v>8</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5983</v>
+      </c>
+      <c r="B55" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55">
+        <v>75</v>
+      </c>
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>6011</v>
+      </c>
+      <c r="B56" t="s">
+        <v>170</v>
+      </c>
+      <c r="C56">
+        <v>75</v>
+      </c>
+      <c r="E56">
+        <v>8</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>6020</v>
+      </c>
+      <c r="B57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57">
+        <v>25</v>
+      </c>
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>6039</v>
+      </c>
+      <c r="B58" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58">
+        <v>35</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>5646</v>
+      </c>
+      <c r="B59" t="s">
+        <v>401</v>
+      </c>
+      <c r="C59">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>400</v>
+      </c>
+      <c r="E59">
+        <v>9</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>5647</v>
+      </c>
+      <c r="B60" t="s">
+        <v>399</v>
+      </c>
+      <c r="C60">
+        <v>75</v>
+      </c>
+      <c r="D60" t="s">
+        <v>398</v>
+      </c>
+      <c r="E60">
+        <v>9</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>5648</v>
+      </c>
+      <c r="B61" t="s">
+        <v>397</v>
+      </c>
+      <c r="C61">
+        <v>125</v>
+      </c>
+      <c r="D61" t="s">
+        <v>396</v>
+      </c>
+      <c r="E61">
+        <v>9</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>5697</v>
+      </c>
+      <c r="B62" t="s">
+        <v>395</v>
+      </c>
+      <c r="C62">
+        <v>50</v>
+      </c>
+      <c r="D62" t="s">
+        <v>394</v>
+      </c>
+      <c r="E62">
+        <v>9</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>5868</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63">
+        <v>125</v>
+      </c>
+      <c r="E63">
+        <v>9</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>5835</v>
+      </c>
+      <c r="B64" t="s">
+        <v>393</v>
+      </c>
+      <c r="C64">
+        <v>25</v>
+      </c>
+      <c r="D64" t="s">
+        <v>392</v>
+      </c>
+      <c r="E64">
+        <v>9</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>5836</v>
+      </c>
+      <c r="B65" t="s">
+        <v>391</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
+        <v>390</v>
+      </c>
+      <c r="E65">
+        <v>9</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>5837</v>
+      </c>
+      <c r="B66" t="s">
+        <v>389</v>
+      </c>
+      <c r="C66">
+        <v>65</v>
+      </c>
+      <c r="D66" t="s">
+        <v>388</v>
+      </c>
+      <c r="E66">
+        <v>9</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>5838</v>
+      </c>
+      <c r="B67" t="s">
+        <v>387</v>
+      </c>
+      <c r="C67">
+        <v>35</v>
+      </c>
+      <c r="D67" t="s">
+        <v>386</v>
+      </c>
+      <c r="E67">
+        <v>9</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>5839</v>
+      </c>
+      <c r="B68" t="s">
+        <v>385</v>
+      </c>
+      <c r="C68">
+        <v>35</v>
+      </c>
+      <c r="D68" t="s">
+        <v>384</v>
+      </c>
+      <c r="E68">
+        <v>9</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>5701</v>
+      </c>
+      <c r="B69" t="s">
+        <v>383</v>
+      </c>
+      <c r="C69">
+        <v>125</v>
+      </c>
+      <c r="D69" t="s">
+        <v>382</v>
+      </c>
+      <c r="E69">
+        <v>14</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>5702</v>
+      </c>
+      <c r="B70" t="s">
+        <v>381</v>
+      </c>
+      <c r="C70">
+        <v>125</v>
+      </c>
+      <c r="D70" t="s">
+        <v>380</v>
+      </c>
+      <c r="E70">
+        <v>14</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5722</v>
+      </c>
+      <c r="B71" t="s">
+        <v>379</v>
+      </c>
+      <c r="C71">
+        <v>75</v>
+      </c>
+      <c r="D71" t="s">
+        <v>378</v>
+      </c>
+      <c r="E71">
+        <v>14</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>5872</v>
+      </c>
+      <c r="B72" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72">
+        <v>25</v>
+      </c>
+      <c r="E72">
+        <v>14</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>5874</v>
+      </c>
+      <c r="B73" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>47</v>
+      </c>
+      <c r="E73">
+        <v>14</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>5875</v>
+      </c>
+      <c r="B74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74">
+        <v>25</v>
+      </c>
+      <c r="E74">
+        <v>14</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>5881</v>
+      </c>
+      <c r="B75" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75">
+        <v>90</v>
+      </c>
+      <c r="E75">
+        <v>14</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>5884</v>
+      </c>
+      <c r="B76" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76">
+        <v>65</v>
+      </c>
+      <c r="E76">
+        <v>14</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>5892</v>
+      </c>
+      <c r="B77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77">
+        <v>125</v>
+      </c>
+      <c r="D77" t="s">
+        <v>377</v>
+      </c>
+      <c r="E77">
+        <v>14</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>5903</v>
+      </c>
+      <c r="B78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78">
+        <v>165</v>
+      </c>
+      <c r="E78">
+        <v>14</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>5905</v>
+      </c>
+      <c r="B79" t="s">
+        <v>67</v>
+      </c>
+      <c r="C79">
+        <v>170</v>
+      </c>
+      <c r="E79">
+        <v>14</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>5917</v>
+      </c>
+      <c r="B80" t="s">
+        <v>76</v>
+      </c>
+      <c r="C80">
+        <v>75</v>
+      </c>
+      <c r="E80">
+        <v>14</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>5938</v>
+      </c>
+      <c r="B81" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81">
+        <v>110</v>
+      </c>
+      <c r="E81">
+        <v>14</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>5973</v>
+      </c>
+      <c r="B82" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82">
+        <v>50</v>
+      </c>
+      <c r="D82" t="s">
+        <v>376</v>
+      </c>
+      <c r="E82">
+        <v>14</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>6050</v>
+      </c>
+      <c r="B83" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83">
+        <v>45</v>
+      </c>
+      <c r="E83">
+        <v>14</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>5792</v>
+      </c>
+      <c r="B84" t="s">
+        <v>375</v>
+      </c>
+      <c r="C84">
+        <v>75</v>
+      </c>
+      <c r="D84" t="s">
+        <v>374</v>
+      </c>
+      <c r="E84">
+        <v>14</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>5929</v>
+      </c>
+      <c r="B85" t="s">
+        <v>31</v>
+      </c>
+      <c r="C85">
+        <v>30</v>
+      </c>
+      <c r="E85">
+        <v>14</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>5967</v>
+      </c>
+      <c r="B86" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86">
+        <v>55</v>
+      </c>
+      <c r="E86">
+        <v>14</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>5984</v>
+      </c>
+      <c r="B87" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87">
+        <v>100</v>
+      </c>
+      <c r="E87">
+        <v>14</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>5986</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88">
+        <v>150</v>
+      </c>
+      <c r="E88">
+        <v>14</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>6000</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89">
+        <v>35</v>
+      </c>
+      <c r="E89">
+        <v>14</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>6032</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90">
+        <v>70</v>
+      </c>
+      <c r="E90">
+        <v>14</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>6074</v>
+      </c>
+      <c r="B91" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91">
+        <v>75</v>
+      </c>
+      <c r="E91">
+        <v>14</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>5871</v>
+      </c>
+      <c r="B92" t="s">
+        <v>202</v>
+      </c>
+      <c r="C92">
+        <v>75</v>
+      </c>
+      <c r="E92">
+        <v>14</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>5882</v>
+      </c>
+      <c r="B93" t="s">
+        <v>119</v>
+      </c>
+      <c r="C93">
+        <v>50</v>
+      </c>
+      <c r="E93">
+        <v>14</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>5889</v>
+      </c>
+      <c r="B94" t="s">
+        <v>132</v>
+      </c>
+      <c r="C94">
+        <v>25</v>
+      </c>
+      <c r="E94">
+        <v>14</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>5966</v>
+      </c>
+      <c r="B95" t="s">
+        <v>113</v>
+      </c>
+      <c r="C95">
+        <v>25</v>
+      </c>
+      <c r="D95" t="s">
+        <v>114</v>
+      </c>
+      <c r="E95">
+        <v>14</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>6013</v>
+      </c>
+      <c r="B96" t="s">
+        <v>171</v>
+      </c>
+      <c r="C96">
+        <v>55</v>
+      </c>
+      <c r="E96">
+        <v>14</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>6029</v>
+      </c>
+      <c r="B97" t="s">
+        <v>120</v>
+      </c>
+      <c r="C97">
+        <v>50</v>
+      </c>
+      <c r="E97">
+        <v>14</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>6031</v>
+      </c>
+      <c r="B98" t="s">
+        <v>122</v>
+      </c>
+      <c r="C98">
+        <v>75</v>
+      </c>
+      <c r="E98">
+        <v>14</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>6049</v>
+      </c>
+      <c r="B99" t="s">
+        <v>163</v>
+      </c>
+      <c r="C99">
+        <v>25</v>
+      </c>
+      <c r="E99">
+        <v>14</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added description of magic items
</commit_message>
<xml_diff>
--- a/resources/db/MagicItems.xlsx
+++ b/resources/db/MagicItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00335357-5A7A-4929-B061-F66EF2AE2C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F59D37D-1A7E-4127-8E39-5CCAEB31C9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="437">
   <si>
     <t>id</t>
   </si>
@@ -1320,6 +1320,39 @@
   </si>
   <si>
     <t>Bluttrinker</t>
+  </si>
+  <si>
+    <t>+1 Attacke. Bei Treffer Moralwurf, sonst keine Nahkampfattacken in dieser Runde.</t>
+  </si>
+  <si>
+    <t>RW von 3+, -1 auf alle Trefferwürfe auf den Träger</t>
+  </si>
+  <si>
+    <t>Der Ammulettträger gewinnt zu Beginn jedes seiner Spielzüge 1 LP zurück</t>
+  </si>
+  <si>
+    <t>Explodiert bei Tod. Jeder im Umkreis erhält einen Treffer mit Stärke W6 plus Stärke des Trägers. Schaden W6</t>
+  </si>
+  <si>
+    <t>Reflektiert verlorene LP bei 4+ auf den Verursacher. Kein RW.</t>
+  </si>
+  <si>
+    <t>1x pro Magiephase ein Magie Bann bei 4+</t>
+  </si>
+  <si>
+    <t>1x pro Magiephase eine Energiekarte oder ein Magie Bann</t>
+  </si>
+  <si>
+    <t>+2 Stärke, nicht zuletzt zuschlagen, alle automatische Treffer wenn erste Attacke trifft</t>
+  </si>
+  <si>
+    <t>RW nur magische Rüstungen. 1x pro Spiel als erster Angreifen und +W6 Attacken</t>
+  </si>
+  <si>
+    <t>Parriert eine Attacke eines Gegners. RW: -3</t>
+  </si>
+  <si>
+    <t>Treffer verwunden automatisch. 1x pro Spiel +W6 Treffer der Stärke 6</t>
   </si>
 </sst>
 </file>
@@ -1367,10 +1400,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -11524,11 +11558,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1508439D-2206-4762-B104-9E5E275BF891}">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11703,6 +11737,9 @@
       <c r="C7">
         <v>25</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>426</v>
+      </c>
       <c r="E7">
         <v>5</v>
       </c>
@@ -11726,6 +11763,9 @@
       <c r="C8">
         <v>60</v>
       </c>
+      <c r="D8" t="s">
+        <v>427</v>
+      </c>
       <c r="E8">
         <v>5</v>
       </c>
@@ -11801,6 +11841,9 @@
       <c r="C11">
         <v>25</v>
       </c>
+      <c r="D11" t="s">
+        <v>428</v>
+      </c>
       <c r="E11">
         <v>5</v>
       </c>
@@ -11824,6 +11867,9 @@
       <c r="C12">
         <v>25</v>
       </c>
+      <c r="D12" t="s">
+        <v>429</v>
+      </c>
       <c r="E12">
         <v>5</v>
       </c>
@@ -11847,6 +11893,9 @@
       <c r="C13">
         <v>50</v>
       </c>
+      <c r="D13" t="s">
+        <v>430</v>
+      </c>
       <c r="E13">
         <v>5</v>
       </c>
@@ -11870,6 +11919,9 @@
       <c r="C14">
         <v>25</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>431</v>
+      </c>
       <c r="E14">
         <v>5</v>
       </c>
@@ -11893,6 +11945,9 @@
       <c r="C15">
         <v>50</v>
       </c>
+      <c r="D15" t="s">
+        <v>432</v>
+      </c>
       <c r="E15">
         <v>5</v>
       </c>
@@ -11968,6 +12023,9 @@
       <c r="C18">
         <v>65</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>433</v>
+      </c>
       <c r="E18">
         <v>7</v>
       </c>
@@ -11991,6 +12049,9 @@
       <c r="C19">
         <v>60</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>434</v>
+      </c>
       <c r="E19">
         <v>7</v>
       </c>
@@ -12014,6 +12075,9 @@
       <c r="C20">
         <v>50</v>
       </c>
+      <c r="D20" t="s">
+        <v>435</v>
+      </c>
       <c r="E20">
         <v>7</v>
       </c>
@@ -12037,6 +12101,9 @@
       <c r="C21">
         <v>100</v>
       </c>
+      <c r="D21" t="s">
+        <v>436</v>
+      </c>
       <c r="E21">
         <v>7</v>
       </c>
@@ -13916,6 +13983,29 @@
         <v>1</v>
       </c>
       <c r="H99" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>5954</v>
+      </c>
+      <c r="B100" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100">
+        <v>125</v>
+      </c>
+      <c r="E100">
+        <v>-1</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed mount save of Tyrion
</commit_message>
<xml_diff>
--- a/resources/db/MagicItems.xlsx
+++ b/resources/db/MagicItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F59D37D-1A7E-4127-8E39-5CCAEB31C9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6816F4B1-F239-42FE-B490-3E546803016B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="441">
   <si>
     <t>id</t>
   </si>
@@ -1353,6 +1353,18 @@
   </si>
   <si>
     <t>Treffer verwunden automatisch. 1x pro Spiel +W6 Treffer der Stärke 6</t>
+  </si>
+  <si>
+    <t>+3 Stärke, Schaden W3, automatischer Schaden gegen Dämonen, 1x pro Spiel Feuerstrahl</t>
+  </si>
+  <si>
+    <t>+3 Stärke, RW: keiner</t>
+  </si>
+  <si>
+    <t>Speichert drei Zaubersprüche</t>
+  </si>
+  <si>
+    <t>Reichweite: 36", Stärke: 6 -1 pro Glied, Paniktest für Dunkelelfen</t>
   </si>
 </sst>
 </file>
@@ -11562,7 +11574,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12127,6 +12139,9 @@
       <c r="C22">
         <v>125</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="E22">
         <v>7</v>
       </c>
@@ -12150,6 +12165,9 @@
       <c r="C23">
         <v>60</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>438</v>
+      </c>
       <c r="E23">
         <v>7</v>
       </c>
@@ -12173,6 +12191,9 @@
       <c r="C24">
         <v>50</v>
       </c>
+      <c r="D24" t="s">
+        <v>439</v>
+      </c>
       <c r="E24">
         <v>7</v>
       </c>
@@ -12195,6 +12216,9 @@
       </c>
       <c r="C25">
         <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>440</v>
       </c>
       <c r="E25">
         <v>7</v>

</xml_diff>

<commit_message>
Updated description of more magic items
</commit_message>
<xml_diff>
--- a/resources/db/MagicItems.xlsx
+++ b/resources/db/MagicItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173FD391-0CDC-41A3-8C2A-3BFAF6F73CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE5A900-E2E5-4CBA-8FE9-8C4CDB794598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2B0158EC-1480-4303-8C84-1C4FD7BBF834}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Magic Items" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Magic Items'!$A$1:$I$100</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Unique items 2'!$A$1:$J$182</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="484">
   <si>
     <t>id</t>
   </si>
@@ -1476,6 +1477,24 @@
   </si>
   <si>
     <t>Ranged_Weapon</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Einheiten in 12" Umkreis sammeln sich automatisch</t>
+  </si>
+  <si>
+    <t>Verleiht Träger Magiestufe 3. Bei jedem Zauber einen Moraltest, sonst bis zur nächsten Magiephase aussetzen.</t>
+  </si>
+  <si>
+    <t>+2 auf Stärke, nicht zuletzt zuschlagen, 2 Würfel pro Treffer- und Schadenswurf besseres Ergebnis zählt, 2 Würfel für Rettungswurf der Gegner schlechteres Ergebnis zählt</t>
+  </si>
+  <si>
+    <t>Auswahl aus drei Versen: der Wiedergeburt, der Flammenden Ewigkeit, der Zerstörung</t>
+  </si>
+  <si>
+    <t>+1 auf KG, W und Stärke. Attakiert als Erster. Nur magische Rüstungen</t>
   </si>
 </sst>
 </file>
@@ -11685,7 +11704,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11719,22 +11738,25 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6002</v>
+        <v>5954</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="C2">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
-        <v>427</v>
+        <v>480</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -11743,28 +11765,28 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("UPDATE ",H2," SET description = '",D2,"' WHERE id = ",A2,";")</f>
-        <v>UPDATE Armor SET description = 'RW von 3+, -1 auf alle Trefferwürfe auf den Träger' WHERE id = 6002;</v>
+        <v>UPDATE Misc SET description = 'Verleiht Träger Magiestufe 3. Bei jedem Zauber einen Moraltest, sonst bis zur nächsten Magiephase aussetzen.' WHERE id = 5954;</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5793</v>
+        <v>6002</v>
       </c>
       <c r="B3" t="s">
-        <v>411</v>
+        <v>24</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -11776,85 +11798,85 @@
         <v>9</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I66" si="0">CONCATENATE("UPDATE ",H3," SET description = '",D3,"' WHERE id = ",A3,";")</f>
-        <v>UPDATE Armor SET description = '-1 auf Stärke des Gegner, wenn er keine magische Waffe trägt.' WHERE id = 5793;</v>
+        <f>CONCATENATE("UPDATE ",H3," SET description = '",D3,"' WHERE id = ",A3,";")</f>
+        <v>UPDATE Armor SET description = 'RW von 3+, -1 auf alle Trefferwürfe auf den Träger' WHERE id = 6002;</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5959</v>
+        <v>5655</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>425</v>
       </c>
       <c r="C4">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'RW: 2+, Zweiter unmodifizierter RW: 4+, Immun gegen Feuer' WHERE id = 5959;</v>
+        <f>CONCATENATE("UPDATE ",H4," SET description = '",D4,"' WHERE id = ",A4,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Jede Verletzung kostet zusätzlich 1 Stärkepunkt.' WHERE id = 5655;</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5979</v>
+        <v>5656</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>423</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'Moraltest wiederholen' WHERE id = 5979;</v>
+        <f>CONCATENATE("UPDATE ",H5," SET description = '",D5,"' WHERE id = ",A5,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Jede Treffer raubt bei 4+ einen magische Gegenstand oder Zauberspruch.' WHERE id = 5656;</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5998</v>
+        <v>5665</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>421</v>
       </c>
       <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>443</v>
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>420</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -11863,88 +11885,88 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = '+2 auf RW gegen Beschuß, +1 auf RW im Nahkamp, Immun gegen Gift' WHERE id = 5998;</v>
+        <f>CONCATENATE("UPDATE ",H6," SET description = '",D6,"' WHERE id = ",A6,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Jede Verletztung kostet einen Punkt von KG und BF des Opfers.' WHERE id = 5665;</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6005</v>
+        <v>5716</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>379</v>
       </c>
       <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>444</v>
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>378</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'RW: 2+, RW nie schlechter als 5+, Immun gegen Dracheodem' WHERE id = 6005;</v>
+        <f>CONCATENATE("UPDATE ",H7," SET description = '",D7,"' WHERE id = ",A7,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5716;</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6017</v>
+        <v>5896</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>419</v>
       </c>
       <c r="C8">
-        <v>45</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>445</v>
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>418</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = '-2 auf Stärke der Gegner. Bannt automatisch ersten Zauberspruch gegen den Träger.' WHERE id = 6017;</v>
+        <f>CONCATENATE("UPDATE ",H8," SET description = '",D8,"' WHERE id = ",A8,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Opfer geköpft bei Schadenswurf von 6. Nur magische Rüstungen.' WHERE id = 5896;</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5792</v>
+        <v>5912</v>
       </c>
       <c r="B9" t="s">
-        <v>375</v>
+        <v>72</v>
       </c>
       <c r="C9">
-        <v>75</v>
-      </c>
-      <c r="D9" t="s">
-        <v>374</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>426</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -11953,85 +11975,88 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'RW von 2+, zweiter unmodifizierter RW von 4+.' WHERE id = 5792;</v>
+        <f>CONCATENATE("UPDATE ",H9," SET description = '",D9,"' WHERE id = ",A9,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+1 Attacke. Bei Treffer Moralwurf, sonst keine Nahkampfattacken in dieser Runde.' WHERE id = 5912;</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5929</v>
+        <v>5937</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>415</v>
       </c>
       <c r="C10">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>414</v>
       </c>
       <c r="E10">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = '' WHERE id = 5929;</v>
+        <f>CONCATENATE("UPDATE ",H10," SET description = '",D10,"' WHERE id = ",A10,";")</f>
+        <v>UPDATE Misc SET description = '+3 auf Stärke für einen Spielzug' WHERE id = 5937;</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5967</v>
+        <v>5961</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="C11">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>471</v>
+        <v>428</v>
       </c>
       <c r="E11">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'Steinrune (+1 auf RW), Eisenrune (+1 auf W)' WHERE id = 5967;</v>
+        <f>CONCATENATE("UPDATE ",H11," SET description = '",D11,"' WHERE id = ",A11,";")</f>
+        <v>UPDATE Misc SET description = 'Der Ammulettträger gewinnt zu Beginn jedes seiner Spielzüge 1 LP zurück' WHERE id = 5961;</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5984</v>
+        <v>5980</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="C12">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>470</v>
+        <v>429</v>
       </c>
       <c r="E12">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -12040,232 +12065,238 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'Adamant Meisterrund (+2 auf RW), Widerstandsrune (wiederholter RW mit 4+)' WHERE id = 5984;</v>
+        <f>CONCATENATE("UPDATE ",H12," SET description = '",D12,"' WHERE id = ",A12,";")</f>
+        <v>UPDATE Misc SET description = 'Explodiert bei Tod. Jeder im Umkreis erhält einen Treffer mit Stärke W6 plus Stärke des Trägers. Schaden W6' WHERE id = 5980;</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5986</v>
+        <v>6009</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="C13">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>472</v>
+        <v>430</v>
       </c>
       <c r="E13">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'Adamant Meisterrund (+2 auf RW), Widerstandsrune (wiederholter RW mit 4+), Magieschluckende Rune (automatischer Magie Bann)' WHERE id = 5986;</v>
+        <f>CONCATENATE("UPDATE ",H13," SET description = '",D13,"' WHERE id = ",A13,";")</f>
+        <v>UPDATE Misc SET description = 'Reflektiert verlorene LP bei 4+ auf den Verursacher. Kein RW.' WHERE id = 6009;</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6000</v>
+        <v>6036</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="C14">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>431</v>
       </c>
       <c r="E14">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = '' WHERE id = 6000;</v>
+        <f>CONCATENATE("UPDATE ",H14," SET description = '",D14,"' WHERE id = ",A14,";")</f>
+        <v>UPDATE Misc SET description = '1x pro Magiephase ein Magie Bann bei 4+' WHERE id = 6036;</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6032</v>
+        <v>6065</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
       <c r="C15">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>473</v>
+        <v>432</v>
       </c>
       <c r="E15">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = 'Meisterrune der Vergeltung (reflektiert Nahkampfschaden bei 4+), Schmiedefeuerrune (Immun gegen Feuer und Hitze), Glücksrune (Würfelwurf wiederholen)' WHERE id = 6032;</v>
+        <f>CONCATENATE("UPDATE ",H15," SET description = '",D15,"' WHERE id = ",A15,";")</f>
+        <v>UPDATE Misc SET description = '1x pro Magiephase eine Energiekarte oder ein Magie Bann' WHERE id = 6065;</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6074</v>
+        <v>5840</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>417</v>
       </c>
       <c r="C16">
-        <v>75</v>
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>416</v>
       </c>
       <c r="E16">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Armor SET description = '' WHERE id = 6074;</v>
+        <f>CONCATENATE("UPDATE ",H16," SET description = '",D16,"' WHERE id = ",A16,";")</f>
+        <v>UPDATE Standard SET description = 'Ignoriert die Auswirkung von Blödheit. Nur für Echsenreiter.' WHERE id = 5840;</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>6076</v>
+        <v>5793</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>411</v>
       </c>
       <c r="C17">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="E17">
         <v>7</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Instrument SET description = 'Einmal pro Schlacht entweder 2x Schießen oder 2x Attackieren' WHERE id = 6076;</v>
+        <f>CONCATENATE("UPDATE ",H17," SET description = '",D17,"' WHERE id = ",A17,";")</f>
+        <v>UPDATE Armor SET description = '-1 auf Stärke des Gegner, wenn er keine magische Waffe trägt.' WHERE id = 5793;</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5642</v>
+        <v>5959</v>
       </c>
       <c r="B18" t="s">
-        <v>407</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>476</v>
+        <v>9</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Jeder Treffer verletzt automatisch. RW nur für magische Rüstungen.' WHERE id = 5642;</v>
+        <f>CONCATENATE("UPDATE ",H18," SET description = '",D18,"' WHERE id = ",A18,";")</f>
+        <v>UPDATE Armor SET description = 'RW: 2+, Zweiter unmodifizierter RW: 4+, Immun gegen Feuer' WHERE id = 5959;</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5659</v>
+        <v>5979</v>
       </c>
       <c r="B19" t="s">
-        <v>405</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>404</v>
+        <v>442</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>476</v>
+        <v>9</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Kein Rettungswurf erlaubt. Untote verlieren 2 Lebenspunkte.' WHERE id = 5659;</v>
+        <f>CONCATENATE("UPDATE ",H19," SET description = '",D19,"' WHERE id = ",A19,";")</f>
+        <v>UPDATE Armor SET description = 'Moraltest wiederholen' WHERE id = 5979;</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5692</v>
+        <v>5998</v>
       </c>
       <c r="B20" t="s">
-        <v>403</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>402</v>
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>443</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -12274,88 +12305,88 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>476</v>
+        <v>9</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Trefferwurf darf einmal wiederholt werden.' WHERE id = 5692;</v>
+        <f>CONCATENATE("UPDATE ",H20," SET description = '",D20,"' WHERE id = ",A20,";")</f>
+        <v>UPDATE Armor SET description = '+2 auf RW gegen Beschuß, +1 auf RW im Nahkamp, Immun gegen Gift' WHERE id = 5998;</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5718</v>
+        <v>6005</v>
       </c>
       <c r="B21" t="s">
-        <v>379</v>
+        <v>27</v>
       </c>
       <c r="C21">
-        <v>75</v>
-      </c>
-      <c r="D21" t="s">
-        <v>378</v>
+        <v>30</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>444</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>476</v>
+        <v>9</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5718;</v>
+        <f>CONCATENATE("UPDATE ",H21," SET description = '",D21,"' WHERE id = ",A21,";")</f>
+        <v>UPDATE Armor SET description = 'RW: 2+, RW nie schlechter als 5+, Immun gegen Dracheodem' WHERE id = 6005;</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>5890</v>
+        <v>6017</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C22">
-        <v>100</v>
-      </c>
-      <c r="D22" t="s">
-        <v>457</v>
+        <v>45</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>445</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>476</v>
+        <v>9</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'nur magische Rüstungen, Schaden: W6+1' WHERE id = 5890;</v>
+        <f>CONCATENATE("UPDATE ",H22," SET description = '",D22,"' WHERE id = ",A22,";")</f>
+        <v>UPDATE Armor SET description = '-2 auf Stärke der Gegner. Bannt automatisch ersten Zauberspruch gegen den Träger.' WHERE id = 6017;</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5936</v>
+        <v>6076</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C23">
-        <v>80</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>458</v>
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
       </c>
       <c r="E23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -12364,28 +12395,28 @@
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>476</v>
+        <v>40</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+2 auf Stärke, +1 auf Stärke wenn Kriegsaltar beschädigt, kein Zaubern mehr wenn Kriesaltar zerstört' WHERE id = 5936;</v>
+        <f>CONCATENATE("UPDATE ",H23," SET description = '",D23,"' WHERE id = ",A23,";")</f>
+        <v>UPDATE Instrument SET description = 'Einmal pro Schlacht entweder 2x Schießen oder 2x Attackieren' WHERE id = 6076;</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5952</v>
+        <v>5717</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>379</v>
       </c>
       <c r="C24">
         <v>75</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>459</v>
+      <c r="D24" t="s">
+        <v>378</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -12397,25 +12428,25 @@
         <v>476</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Zaubersprüche können nicht gebannt werden. Bei 1-2 auf W6 verbraucht' WHERE id = 5952;</v>
+        <f>CONCATENATE("UPDATE ",H24," SET description = '",D24,"' WHERE id = ",A24,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5717;</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>5646</v>
+        <v>5733</v>
       </c>
       <c r="B25" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
       <c r="C25">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="E25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -12427,25 +12458,25 @@
         <v>476</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Erster Verpatzter Stänkereitest kann ignoriert werden. Nur für Orks und Wildorks' WHERE id = 5646;</v>
+        <f>CONCATENATE("UPDATE ",H25," SET description = '",D25,"' WHERE id = ",A25,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+2 Stärke beim Angriff. Trifft automatisch. Spezialattacke' WHERE id = 5733;</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5647</v>
+        <v>5869</v>
       </c>
       <c r="B26" t="s">
-        <v>399</v>
+        <v>43</v>
       </c>
       <c r="C26">
-        <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>398</v>
+        <v>65</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>433</v>
       </c>
       <c r="E26">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -12457,28 +12488,28 @@
         <v>476</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+1 auf Stärke. Pro Mob ein Blitz mit Reichweite: 24", Stärke: 4, RW: keiner.' WHERE id = 5647;</v>
+        <f>CONCATENATE("UPDATE ",H26," SET description = '",D26,"' WHERE id = ",A26,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+2 Stärke, nicht zuletzt zuschlagen, alle automatische Treffer wenn erste Attacke trifft' WHERE id = 5869;</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>5648</v>
+        <v>5899</v>
       </c>
       <c r="B27" t="s">
-        <v>397</v>
+        <v>62</v>
       </c>
       <c r="C27">
-        <v>125</v>
-      </c>
-      <c r="D27" t="s">
-        <v>396</v>
+        <v>60</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>434</v>
       </c>
       <c r="E27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -12487,28 +12518,28 @@
         <v>476</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Träger attackiert immer zuerst. +1 auf KG, S und W, kein RW oder mit -3.' WHERE id = 5648;</v>
+        <f>CONCATENATE("UPDATE ",H27," SET description = '",D27,"' WHERE id = ",A27,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'RW nur magische Rüstungen. 1x pro Spiel als erster Angreifen und +W6 Attacken' WHERE id = 5899;</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>5697</v>
+        <v>5904</v>
       </c>
       <c r="B28" t="s">
-        <v>395</v>
+        <v>66</v>
       </c>
       <c r="C28">
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>394</v>
+        <v>435</v>
       </c>
       <c r="E28">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -12517,22 +12548,25 @@
         <v>476</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Verursacht 2 Schadenspunkte, kein Rettungswurf.' WHERE id = 5697;</v>
+        <f>CONCATENATE("UPDATE ",H28," SET description = '",D28,"' WHERE id = ",A28,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Parriert eine Attacke eines Gegners. RW: -3' WHERE id = 5904;</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>5868</v>
+        <v>5925</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C29">
-        <v>125</v>
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>436</v>
       </c>
       <c r="E29">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -12544,28 +12578,28 @@
         <v>476</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5868;</v>
+        <f>CONCATENATE("UPDATE ",H29," SET description = '",D29,"' WHERE id = ",A29,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Treffer verwunden automatisch. 1x pro Spiel +W6 Treffer der Stärke 6' WHERE id = 5925;</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>5701</v>
+        <v>5932</v>
       </c>
       <c r="B30" t="s">
-        <v>383</v>
+        <v>85</v>
       </c>
       <c r="C30">
         <v>125</v>
       </c>
-      <c r="D30" t="s">
-        <v>382</v>
+      <c r="D30" s="3" t="s">
+        <v>437</v>
       </c>
       <c r="E30">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -12574,25 +12608,25 @@
         <v>476</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Schaden bei 2+, W3 LP, kein RW o. RW:-3. W6 LP gegen Oger u. Trolle.' WHERE id = 5701;</v>
+        <f>CONCATENATE("UPDATE ",H30," SET description = '",D30,"' WHERE id = ",A30,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+3 Stärke, Schaden W3, automatischer Schaden gegen Dämonen, 1x pro Spiel Feuerstrahl' WHERE id = 5932;</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5702</v>
+        <v>5940</v>
       </c>
       <c r="B31" t="s">
-        <v>381</v>
+        <v>96</v>
       </c>
       <c r="C31">
-        <v>125</v>
-      </c>
-      <c r="D31" t="s">
-        <v>380</v>
+        <v>60</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="E31">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -12604,28 +12638,28 @@
         <v>476</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Schaden bei 2+, W3 LP, kein RW o. RW:-3. Drachen u. Dämonen W6 LP.' WHERE id = 5702;</v>
+        <f>CONCATENATE("UPDATE ",H31," SET description = '",D31,"' WHERE id = ",A31,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+3 Stärke, RW: keiner' WHERE id = 5940;</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>5722</v>
+        <v>6056</v>
       </c>
       <c r="B32" t="s">
-        <v>379</v>
+        <v>94</v>
       </c>
       <c r="C32">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>378</v>
+        <v>439</v>
       </c>
       <c r="E32">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -12634,22 +12668,25 @@
         <v>476</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5722;</v>
+        <f>CONCATENATE("UPDATE ",H32," SET description = '",D32,"' WHERE id = ",A32,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Speichert drei Zaubersprüche' WHERE id = 6056;</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>5872</v>
+        <v>5939</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="C33">
-        <v>25</v>
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>446</v>
       </c>
       <c r="E33">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -12658,115 +12695,118 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5872;</v>
+        <f>CONCATENATE("UPDATE ",H33," SET description = '",D33,"' WHERE id = ",A33,";")</f>
+        <v>UPDATE Misc SET description = 'Heilt zu Beginn des Spielzugs einen Charater in 12" Umkreis bei 4+ einen LP' WHERE id = 5939;</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>5874</v>
+        <v>5989</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>154</v>
       </c>
       <c r="C34">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>447</v>
       </c>
       <c r="E34">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+1 auf Stärke und Attacken.' WHERE id = 5874;</v>
+        <f>CONCATENATE("UPDATE ",H34," SET description = '",D34,"' WHERE id = ",A34,";")</f>
+        <v>UPDATE Misc SET description = '1x pro Spiel +W6 Magiekarten. Danach werden die Profilewerte von Teclis halbiert.' WHERE id = 5989;</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>5875</v>
+        <v>5995</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="C35">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="E35">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Meisterrune der Flinkheit. Waffenträger schlägt immer zuerst zu.' WHERE id = 5875;</v>
+        <f>CONCATENATE("UPDATE ",H35," SET description = '",D35,"' WHERE id = ",A35,";")</f>
+        <v>UPDATE Misc SET description = 'Alle erfolgreichen Treffer- und Schadenswürfe der Gegner müssen wiederholt werden' WHERE id = 5995;</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>5881</v>
+        <v>6007</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="C36">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="E36">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Zweihändige Axt, Paraderune (-1 auf Attacken von Gegner), Schadensrune (Schaden: W6)' WHERE id = 5881;</v>
+        <f>CONCATENATE("UPDATE ",H36," SET description = '",D36,"' WHERE id = ",A36,";")</f>
+        <v>UPDATE Misc SET description = 'Zweiter unmodifzierter RW von 4+' WHERE id = 6007;</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>5884</v>
+        <v>6028</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="C37">
-        <v>65</v>
+        <v>50</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="E37">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -12775,28 +12815,28 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5884;</v>
+        <f>CONCATENATE("UPDATE ",H37," SET description = '",D37,"' WHERE id = ",A37,";")</f>
+        <v>UPDATE Misc SET description = '4+ Rettungswurf gegen Zaubersprüche. Bei Tod automatische Wiederbelebung mit 1 LP' WHERE id = 6028;</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>5892</v>
+        <v>6030</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="C38">
-        <v>125</v>
-      </c>
-      <c r="D38" t="s">
-        <v>377</v>
+        <v>15</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="E38">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -12805,85 +12845,88 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Schadenswurf ist immer 2+. Nur magische Rüstungen mit -3 auf RW. Jede Verletztung kostet W3 LP. Drachen und Dämonen verlieren W6 LP.' WHERE id = 5892;</v>
+        <f>CONCATENATE("UPDATE ",H38," SET description = '",D38,"' WHERE id = ",A38,";")</f>
+        <v>UPDATE Misc SET description = '1x pro Spiel +W6 zusätzliche Attacken für Imriks Drachen' WHERE id = 6030;</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>5903</v>
+        <v>6041</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="C39">
-        <v>165</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>467</v>
+        <v>125</v>
+      </c>
+      <c r="D39" t="s">
+        <v>452</v>
       </c>
       <c r="E39">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+1 auf Attacken, Stärke: 10, automatischer Schaden wenn Gegner durch Feuer verwundbar, Schaden: W6' WHERE id = 5903;</v>
+        <f>CONCATENATE("UPDATE ",H39," SET description = '",D39,"' WHERE id = ",A39,";")</f>
+        <v>UPDATE Misc SET description = 'Erhöhte wie Magiestufe von 4 auf 5' WHERE id = 6041;</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>5905</v>
+        <v>6053</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="C40">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="E40">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Meisterrune des Todes (Jede Verletzung tötet), Kampfgeschickrune (+1 auf KG), Kraftrune (Stärke x2 gegen Gegner mit mehr Widerstand)' WHERE id = 5905;</v>
+        <f>CONCATENATE("UPDATE ",H40," SET description = '",D40,"' WHERE id = ",A40,";")</f>
+        <v>UPDATE Misc SET description = 'Verdoppelte Bewegung. Einzelmodelle können Nahkampf verlassen' WHERE id = 6053;</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>5917</v>
+        <v>6055</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>172</v>
       </c>
       <c r="C41">
-        <v>75</v>
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>454</v>
       </c>
       <c r="E41">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -12892,55 +12935,58 @@
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5917;</v>
+        <f>CONCATENATE("UPDATE ",H41," SET description = '",D41,"' WHERE id = ",A41,";")</f>
+        <v>UPDATE Misc SET description = 'Verstärkt jeden Zauberspruch des Trägers um eine Energiekarte' WHERE id = 6055;</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>5938</v>
+        <v>6058</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>175</v>
       </c>
       <c r="C42">
-        <v>110</v>
+        <v>85</v>
+      </c>
+      <c r="D42" t="s">
+        <v>455</v>
       </c>
       <c r="E42">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5938;</v>
+        <f>CONCATENATE("UPDATE ",H42," SET description = '",D42,"' WHERE id = ",A42,";")</f>
+        <v>UPDATE Misc SET description = 'Träger erhält die magischen Fähigkeiten eines Stufe 2 Obermagiers.' WHERE id = 6058;</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>5973</v>
+        <v>6063</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="C43">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>376</v>
+        <v>482</v>
       </c>
       <c r="E43">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -12949,88 +12995,88 @@
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+2 auf Attacken' WHERE id = 5973;</v>
+        <f>CONCATENATE("UPDATE ",H43," SET description = '",D43,"' WHERE id = ",A43,";")</f>
+        <v>UPDATE Misc SET description = 'Auswahl aus drei Versen: der Wiedergeburt, der Flammenden Ewigkeit, der Zerstörung' WHERE id = 6063;</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>6050</v>
+        <v>6071</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
       <c r="C44">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="E44">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Immun gegen Feuer und Hitze, 1x pro Spiel automatischer Magie Bann, normale Bewegung durch schwieriges Gelände' WHERE id = 6050;</v>
+        <f>CONCATENATE("UPDATE ",H44," SET description = '",D44,"' WHERE id = ",A44,";")</f>
+        <v>UPDATE Misc SET description = 'Automatischer Magie Bann oder ein Zauber ohne Energiekarten. 2x einsetzbar.' WHERE id = 6071;</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>5655</v>
+        <v>5908</v>
       </c>
       <c r="B45" t="s">
-        <v>425</v>
+        <v>190</v>
       </c>
       <c r="C45">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>424</v>
+        <v>440</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Jede Verletzung kostet zusätzlich 1 Stärkepunkt.' WHERE id = 5655;</v>
+        <f>CONCATENATE("UPDATE ",H45," SET description = '",D45,"' WHERE id = ",A45,";")</f>
+        <v>UPDATE Ranged_Weapon SET description = 'Reichweite: 36", Stärke: 6 -1 pro Glied, Paniktest für Dunkelelfen' WHERE id = 5908;</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>5656</v>
+        <v>5776</v>
       </c>
       <c r="B46" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="C46">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -13039,58 +13085,58 @@
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>476</v>
+        <v>194</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Jede Treffer raubt bei 4+ einen magische Gegenstand oder Zauberspruch.' WHERE id = 5656;</v>
+        <f>CONCATENATE("UPDATE ",H46," SET description = '",D46,"' WHERE id = ",A46,";")</f>
+        <v>UPDATE Shield SET description = 'Bei eigenem RW, erleidet der Gegner einen Treffer der Stärke 4.' WHERE id = 5776;</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>5665</v>
+        <v>5842</v>
       </c>
       <c r="B47" t="s">
-        <v>421</v>
+        <v>200</v>
       </c>
       <c r="C47">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>420</v>
+        <v>201</v>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>476</v>
+        <v>199</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Jede Verletztung kostet einen Punkt von KG und BF des Opfers.' WHERE id = 5665;</v>
+        <f>CONCATENATE("UPDATE ",H47," SET description = '",D47,"' WHERE id = ",A47,";")</f>
+        <v>UPDATE Standard SET description = 'Gegner muss Moraltest bestehen um Jungferngarde anzugreifen.' WHERE id = 5842;</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>5716</v>
+        <v>5642</v>
       </c>
       <c r="B48" t="s">
-        <v>379</v>
+        <v>407</v>
       </c>
       <c r="C48">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
       <c r="E48">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -13102,25 +13148,25 @@
         <v>476</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5716;</v>
+        <f>CONCATENATE("UPDATE ",H48," SET description = '",D48,"' WHERE id = ",A48,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Jeder Treffer verletzt automatisch. RW nur für magische Rüstungen.' WHERE id = 5642;</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>5896</v>
+        <v>5659</v>
       </c>
       <c r="B49" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="C49">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -13132,25 +13178,25 @@
         <v>476</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Opfer geköpft bei Schadenswurf von 6. Nur magische Rüstungen.' WHERE id = 5896;</v>
+        <f>CONCATENATE("UPDATE ",H49," SET description = '",D49,"' WHERE id = ",A49,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Kein Rettungswurf erlaubt. Untote verlieren 2 Lebenspunkte.' WHERE id = 5659;</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>5912</v>
+        <v>5692</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>403</v>
       </c>
       <c r="C50">
-        <v>25</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>426</v>
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>402</v>
       </c>
       <c r="E50">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -13162,13 +13208,13 @@
         <v>476</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+1 Attacke. Bei Treffer Moralwurf, sonst keine Nahkampfattacken in dieser Runde.' WHERE id = 5912;</v>
+        <f>CONCATENATE("UPDATE ",H50," SET description = '",D50,"' WHERE id = ",A50,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Trefferwurf darf einmal wiederholt werden.' WHERE id = 5692;</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>5717</v>
+        <v>5718</v>
       </c>
       <c r="B51" t="s">
         <v>379</v>
@@ -13180,7 +13226,7 @@
         <v>378</v>
       </c>
       <c r="E51">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -13192,25 +13238,25 @@
         <v>476</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5717;</v>
+        <f>CONCATENATE("UPDATE ",H51," SET description = '",D51,"' WHERE id = ",A51,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5718;</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>5733</v>
+        <v>5890</v>
       </c>
       <c r="B52" t="s">
-        <v>413</v>
+        <v>55</v>
       </c>
       <c r="C52">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>412</v>
+        <v>457</v>
       </c>
       <c r="E52">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -13222,28 +13268,28 @@
         <v>476</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+2 Stärke beim Angriff. Trifft automatisch. Spezialattacke' WHERE id = 5733;</v>
+        <f>CONCATENATE("UPDATE ",H52," SET description = '",D52,"' WHERE id = ",A52,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'nur magische Rüstungen, Schaden: W6+1' WHERE id = 5890;</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>5869</v>
+        <v>5936</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="C53">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>433</v>
+        <v>458</v>
       </c>
       <c r="E53">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -13252,28 +13298,28 @@
         <v>476</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+2 Stärke, nicht zuletzt zuschlagen, alle automatische Treffer wenn erste Attacke trifft' WHERE id = 5869;</v>
+        <f>CONCATENATE("UPDATE ",H53," SET description = '",D53,"' WHERE id = ",A53,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+2 auf Stärke, +1 auf Stärke wenn Kriegsaltar beschädigt, kein Zaubern mehr wenn Kriesaltar zerstört' WHERE id = 5936;</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>5899</v>
+        <v>5952</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="C54">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>434</v>
+        <v>459</v>
       </c>
       <c r="E54">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -13282,25 +13328,25 @@
         <v>476</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'RW nur magische Rüstungen. 1x pro Spiel als erster Angreifen und +W6 Attacken' WHERE id = 5899;</v>
+        <f>CONCATENATE("UPDATE ",H54," SET description = '",D54,"' WHERE id = ",A54,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Zaubersprüche können nicht gebannt werden. Bei 1-2 auf W6 verbraucht' WHERE id = 5952;</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>5904</v>
+        <v>5983</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="C55">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D55" t="s">
-        <v>435</v>
+        <v>461</v>
       </c>
       <c r="E55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -13309,28 +13355,28 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Parriert eine Attacke eines Gegners. RW: -3' WHERE id = 5904;</v>
+        <f>CONCATENATE("UPDATE ",H55," SET description = '",D55,"' WHERE id = ",A55,";")</f>
+        <v>UPDATE Misc SET description = 'Heilt alle LP am Ende der Schuß- und Nahkampfphase' WHERE id = 5983;</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>5925</v>
+        <v>6011</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="C56">
-        <v>100</v>
-      </c>
-      <c r="D56" t="s">
-        <v>436</v>
+        <v>75</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>462</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -13339,58 +13385,58 @@
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Treffer verwunden automatisch. 1x pro Spiel +W6 Treffer der Stärke 6' WHERE id = 5925;</v>
+        <f>CONCATENATE("UPDATE ",H56," SET description = '",D56,"' WHERE id = ",A56,";")</f>
+        <v>UPDATE Misc SET description = '-1 auf Trefferwürfe der Gegener. Magie Bann bei 4+' WHERE id = 6011;</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>5932</v>
+        <v>6020</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="C57">
-        <v>125</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>437</v>
+        <v>25</v>
+      </c>
+      <c r="D57" t="s">
+        <v>463</v>
       </c>
       <c r="E57">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+3 Stärke, Schaden W3, automatischer Schaden gegen Dämonen, 1x pro Spiel Feuerstrahl' WHERE id = 5932;</v>
+        <f>CONCATENATE("UPDATE ",H57," SET description = '",D57,"' WHERE id = ",A57,";")</f>
+        <v>UPDATE Misc SET description = 'Heilt 1 LP zu Beginn des Spielzuges' WHERE id = 6020;</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>5940</v>
+        <v>6039</v>
       </c>
       <c r="B58" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
       <c r="C58">
-        <v>60</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>438</v>
+        <v>35</v>
+      </c>
+      <c r="D58" t="s">
+        <v>464</v>
       </c>
       <c r="E58">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -13399,58 +13445,58 @@
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>476</v>
+        <v>106</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = '+3 Stärke, RW: keiner' WHERE id = 5940;</v>
+        <f>CONCATENATE("UPDATE ",H58," SET description = '",D58,"' WHERE id = ",A58,";")</f>
+        <v>UPDATE Misc SET description = 'Verursacht Entsetzen beim Sturmangriff' WHERE id = 6039;</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>6056</v>
+        <v>5971</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>189</v>
       </c>
       <c r="C59">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D59" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
       <c r="E59">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Melee_Weapon SET description = 'Speichert drei Zaubersprüche' WHERE id = 6056;</v>
+        <f>CONCATENATE("UPDATE ",H59," SET description = '",D59,"' WHERE id = ",A59,";")</f>
+        <v>UPDATE Ranged_Weapon SET description = 'Reichweite: 36", Stärke: 5, Dreifachschuß' WHERE id = 5971;</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>5937</v>
+        <v>5646</v>
       </c>
       <c r="B60" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="C60">
         <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="E60">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -13459,28 +13505,28 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Misc SET description = '+3 auf Stärke für einen Spielzug' WHERE id = 5937;</v>
+        <f>CONCATENATE("UPDATE ",H60," SET description = '",D60,"' WHERE id = ",A60,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Erster Verpatzter Stänkereitest kann ignoriert werden. Nur für Orks und Wildorks' WHERE id = 5646;</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>5961</v>
+        <v>5647</v>
       </c>
       <c r="B61" t="s">
-        <v>110</v>
+        <v>399</v>
       </c>
       <c r="C61">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D61" t="s">
-        <v>428</v>
+        <v>398</v>
       </c>
       <c r="E61">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -13489,28 +13535,28 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Misc SET description = 'Der Ammulettträger gewinnt zu Beginn jedes seiner Spielzüge 1 LP zurück' WHERE id = 5961;</v>
+        <f>CONCATENATE("UPDATE ",H61," SET description = '",D61,"' WHERE id = ",A61,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+1 auf Stärke. Pro Mob ein Blitz mit Reichweite: 24", Stärke: 4, RW: keiner.' WHERE id = 5647;</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>5980</v>
+        <v>5648</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>397</v>
       </c>
       <c r="C62">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="D62" t="s">
-        <v>429</v>
+        <v>396</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -13519,28 +13565,28 @@
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Misc SET description = 'Explodiert bei Tod. Jeder im Umkreis erhält einen Treffer mit Stärke W6 plus Stärke des Trägers. Schaden W6' WHERE id = 5980;</v>
+        <f>CONCATENATE("UPDATE ",H62," SET description = '",D62,"' WHERE id = ",A62,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Träger attackiert immer zuerst. +1 auf KG, S und W, kein RW oder mit -3.' WHERE id = 5648;</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>6009</v>
+        <v>5697</v>
       </c>
       <c r="B63" t="s">
-        <v>168</v>
+        <v>395</v>
       </c>
       <c r="C63">
         <v>50</v>
       </c>
       <c r="D63" t="s">
-        <v>430</v>
+        <v>394</v>
       </c>
       <c r="E63">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -13549,28 +13595,28 @@
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Misc SET description = 'Reflektiert verlorene LP bei 4+ auf den Verursacher. Kein RW.' WHERE id = 6009;</v>
+        <f>CONCATENATE("UPDATE ",H63," SET description = '",D63,"' WHERE id = ",A63,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Verursacht 2 Schadenspunkte, kein Rettungswurf.' WHERE id = 5697;</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>6036</v>
+        <v>5868</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>41</v>
       </c>
       <c r="C64">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>431</v>
+        <v>483</v>
       </c>
       <c r="E64">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -13579,208 +13625,205 @@
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Misc SET description = '1x pro Magiephase ein Magie Bann bei 4+' WHERE id = 6036;</v>
+        <f>CONCATENATE("UPDATE ",H64," SET description = '",D64,"' WHERE id = ",A64,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+1 auf KG, W und Stärke. Attakiert als Erster. Nur magische Rüstungen' WHERE id = 5868;</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>6065</v>
+        <v>5835</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>393</v>
       </c>
       <c r="C65">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="E65">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65">
         <v>1</v>
       </c>
       <c r="H65" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Misc SET description = '1x pro Magiephase eine Energiekarte oder ein Magie Bann' WHERE id = 6065;</v>
+        <f>CONCATENATE("UPDATE ",H65," SET description = '",D65,"' WHERE id = ",A65,";")</f>
+        <v>UPDATE Standard SET description = 'Einheit erhält +1 auf Stärke in der ersten Kampfrunde.' WHERE id = 5835;</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>5939</v>
+        <v>5836</v>
       </c>
       <c r="B66" t="s">
-        <v>173</v>
+        <v>391</v>
       </c>
       <c r="C66">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>446</v>
+        <v>390</v>
       </c>
       <c r="E66">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66">
         <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE Misc SET description = 'Heilt zu Beginn des Spielzugs einen Charater in 12" Umkreis bei 4+ einen LP' WHERE id = 5939;</v>
+        <f>CONCATENATE("UPDATE ",H66," SET description = '",D66,"' WHERE id = ",A66,";")</f>
+        <v>UPDATE Standard SET description = 'Jeden verpatzten Stänkerei-Test wiederholen.' WHERE id = 5836;</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>5989</v>
+        <v>5837</v>
       </c>
       <c r="B67" t="s">
-        <v>154</v>
+        <v>389</v>
       </c>
       <c r="C67">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D67" t="s">
-        <v>447</v>
+        <v>388</v>
       </c>
       <c r="E67">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67">
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I100" si="1">CONCATENATE("UPDATE ",H67," SET description = '",D67,"' WHERE id = ",A67,";")</f>
-        <v>UPDATE Misc SET description = '1x pro Spiel +W6 Magiekarten. Danach werden die Profilewerte von Teclis halbiert.' WHERE id = 5989;</v>
+        <f>CONCATENATE("UPDATE ",H67," SET description = '",D67,"' WHERE id = ",A67,";")</f>
+        <v>UPDATE Standard SET description = 'Magie Bann bei 4+. Zauberer in Base-to-Base-Kontakt platzt der Kopf.' WHERE id = 5837;</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>5995</v>
+        <v>5838</v>
       </c>
       <c r="B68" t="s">
-        <v>159</v>
+        <v>387</v>
       </c>
       <c r="C68">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D68" t="s">
-        <v>448</v>
+        <v>386</v>
       </c>
       <c r="E68">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68">
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Alle erfolgreichen Treffer- und Schadenswürfe der Gegner müssen wiederholt werden' WHERE id = 5995;</v>
+        <f>CONCATENATE("UPDATE ",H68," SET description = '",D68,"' WHERE id = ",A68,";")</f>
+        <v>UPDATE Standard SET description = '-1 auf Beschuß, Nachtgoblins attackieren immer zuerst' WHERE id = 5838;</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>6007</v>
+        <v>5839</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
+        <v>385</v>
       </c>
       <c r="C69">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="D69" t="s">
-        <v>449</v>
+        <v>384</v>
       </c>
       <c r="E69">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69">
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Zweiter unmodifzierter RW von 4+' WHERE id = 6007;</v>
+        <f>CONCATENATE("UPDATE ",H69," SET description = '",D69,"' WHERE id = ",A69,";")</f>
+        <v>UPDATE Standard SET description = 'Verdoppelt Attacken in der ersten Kampfrunde. Nur für Waldgoblins.' WHERE id = 5839;</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>6028</v>
+        <v>5792</v>
       </c>
       <c r="B70" t="s">
-        <v>118</v>
+        <v>375</v>
       </c>
       <c r="C70">
-        <v>50</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>450</v>
+        <v>75</v>
+      </c>
+      <c r="D70" t="s">
+        <v>374</v>
       </c>
       <c r="E70">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70">
         <v>1</v>
       </c>
       <c r="H70" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '4+ Rettungswurf gegen Zaubersprüche. Bei Tod automatische Wiederbelebung mit 1 LP' WHERE id = 6028;</v>
+        <f>CONCATENATE("UPDATE ",H70," SET description = '",D70,"' WHERE id = ",A70,";")</f>
+        <v>UPDATE Armor SET description = 'RW von 2+, zweiter unmodifizierter RW von 4+.' WHERE id = 5792;</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>6030</v>
+        <v>5929</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="C71">
-        <v>15</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>451</v>
+        <v>30</v>
       </c>
       <c r="E71">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -13789,88 +13832,88 @@
         <v>1</v>
       </c>
       <c r="H71" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '1x pro Spiel +W6 zusätzliche Attacken für Imriks Drachen' WHERE id = 6030;</v>
+        <f>CONCATENATE("UPDATE ",H71," SET description = '",D71,"' WHERE id = ",A71,";")</f>
+        <v>UPDATE Armor SET description = '' WHERE id = 5929;</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>6041</v>
+        <v>5967</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>125</v>
+        <v>55</v>
       </c>
       <c r="D72" t="s">
-        <v>452</v>
+        <v>471</v>
       </c>
       <c r="E72">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72">
         <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Erhöhte wie Magiestufe von 4 auf 5' WHERE id = 6041;</v>
+        <f>CONCATENATE("UPDATE ",H72," SET description = '",D72,"' WHERE id = ",A72,";")</f>
+        <v>UPDATE Armor SET description = 'Steinrune (+1 auf RW), Eisenrune (+1 auf W)' WHERE id = 5967;</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>6053</v>
+        <v>5984</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>16</v>
       </c>
       <c r="C73">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="D73" t="s">
-        <v>453</v>
+        <v>470</v>
       </c>
       <c r="E73">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Verdoppelte Bewegung. Einzelmodelle können Nahkampf verlassen' WHERE id = 6053;</v>
+        <f>CONCATENATE("UPDATE ",H73," SET description = '",D73,"' WHERE id = ",A73,";")</f>
+        <v>UPDATE Armor SET description = 'Adamant Meisterrund (+2 auf RW), Widerstandsrune (wiederholter RW mit 4+)' WHERE id = 5984;</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>6055</v>
+        <v>5986</v>
       </c>
       <c r="B74" t="s">
-        <v>172</v>
+        <v>15</v>
       </c>
       <c r="C74">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="D74" t="s">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="E74">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -13879,85 +13922,82 @@
         <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Verstärkt jeden Zauberspruch des Trägers um eine Energiekarte' WHERE id = 6055;</v>
+        <f>CONCATENATE("UPDATE ",H74," SET description = '",D74,"' WHERE id = ",A74,";")</f>
+        <v>UPDATE Armor SET description = 'Adamant Meisterrund (+2 auf RW), Widerstandsrune (wiederholter RW mit 4+), Magieschluckende Rune (automatischer Magie Bann)' WHERE id = 5986;</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>6058</v>
+        <v>6000</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
+        <v>23</v>
       </c>
       <c r="C75">
-        <v>85</v>
-      </c>
-      <c r="D75" t="s">
-        <v>455</v>
+        <v>35</v>
       </c>
       <c r="E75">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75">
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Träger erhält die magischen Fähigkeiten eines Stufe 2 Obermagiers.' WHERE id = 6058;</v>
+        <f>CONCATENATE("UPDATE ",H75," SET description = '",D75,"' WHERE id = ",A75,";")</f>
+        <v>UPDATE Armor SET description = '' WHERE id = 6000;</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>6063</v>
+        <v>6032</v>
       </c>
       <c r="B76" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>25</v>
+        <v>70</v>
+      </c>
+      <c r="D76" t="s">
+        <v>473</v>
       </c>
       <c r="E76">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76">
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '' WHERE id = 6063;</v>
+        <f>CONCATENATE("UPDATE ",H76," SET description = '",D76,"' WHERE id = ",A76,";")</f>
+        <v>UPDATE Armor SET description = 'Meisterrune der Vergeltung (reflektiert Nahkampfschaden bei 4+), Schmiedefeuerrune (Immun gegen Feuer und Hitze), Glücksrune (Würfelwurf wiederholen)' WHERE id = 6032;</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>6071</v>
+        <v>6074</v>
       </c>
       <c r="B77" t="s">
-        <v>167</v>
+        <v>36</v>
       </c>
       <c r="C77">
-        <v>55</v>
-      </c>
-      <c r="D77" t="s">
-        <v>456</v>
+        <v>75</v>
       </c>
       <c r="E77">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -13966,58 +14006,58 @@
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Automatischer Magie Bann oder ein Zauber ohne Energiekarten. 2x einsetzbar.' WHERE id = 6071;</v>
+        <f>CONCATENATE("UPDATE ",H77," SET description = '",D77,"' WHERE id = ",A77,";")</f>
+        <v>UPDATE Armor SET description = '' WHERE id = 6074;</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>5983</v>
+        <v>5701</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>383</v>
       </c>
       <c r="C78">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="D78" t="s">
-        <v>461</v>
+        <v>382</v>
       </c>
       <c r="E78">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78">
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Heilt alle LP am Ende der Schuß- und Nahkampfphase' WHERE id = 5983;</v>
+        <f>CONCATENATE("UPDATE ",H78," SET description = '",D78,"' WHERE id = ",A78,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Schaden bei 2+, W3 LP, kein RW o. RW:-3. W6 LP gegen Oger u. Trolle.' WHERE id = 5701;</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>6011</v>
+        <v>5702</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
+        <v>381</v>
       </c>
       <c r="C79">
-        <v>75</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>462</v>
+        <v>125</v>
+      </c>
+      <c r="D79" t="s">
+        <v>380</v>
       </c>
       <c r="E79">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -14026,28 +14066,28 @@
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '-1 auf Trefferwürfe der Gegener. Magie Bann bei 4+' WHERE id = 6011;</v>
+        <f>CONCATENATE("UPDATE ",H79," SET description = '",D79,"' WHERE id = ",A79,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Schaden bei 2+, W3 LP, kein RW o. RW:-3. Drachen u. Dämonen W6 LP.' WHERE id = 5702;</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>6020</v>
+        <v>5722</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>379</v>
       </c>
       <c r="C80">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D80" t="s">
-        <v>463</v>
+        <v>378</v>
       </c>
       <c r="E80">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -14056,52 +14096,52 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Heilt 1 LP zu Beginn des Spielzuges' WHERE id = 6020;</v>
+        <f>CONCATENATE("UPDATE ",H80," SET description = '",D80,"' WHERE id = ",A80,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Kampfgeschick 10.' WHERE id = 5722;</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>6039</v>
+        <v>5872</v>
       </c>
       <c r="B81" t="s">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="C81">
-        <v>35</v>
-      </c>
-      <c r="D81" t="s">
-        <v>464</v>
+        <v>25</v>
       </c>
       <c r="E81">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81">
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Verursacht Entsetzen beim Sturmangriff' WHERE id = 6039;</v>
+        <f>CONCATENATE("UPDATE ",H81," SET description = '",D81,"' WHERE id = ",A81,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5872;</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>5882</v>
+        <v>5874</v>
       </c>
       <c r="B82" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="C82">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="D82" t="s">
+        <v>47</v>
       </c>
       <c r="E82">
         <v>14</v>
@@ -14113,55 +14153,55 @@
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '' WHERE id = 5882;</v>
+        <f>CONCATENATE("UPDATE ",H82," SET description = '",D82,"' WHERE id = ",A82,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+1 auf Stärke und Attacken.' WHERE id = 5874;</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>5889</v>
+        <v>5875</v>
       </c>
       <c r="B83" t="s">
-        <v>132</v>
+        <v>48</v>
       </c>
       <c r="C83">
         <v>25</v>
       </c>
       <c r="D83" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="E83">
         <v>14</v>
       </c>
       <c r="F83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83">
         <v>1</v>
       </c>
       <c r="H83" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Erzeugt Flammenwall in 6" Entfernung' WHERE id = 5889;</v>
+        <f>CONCATENATE("UPDATE ",H83," SET description = '",D83,"' WHERE id = ",A83,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Meisterrune der Flinkheit. Waffenträger schlägt immer zuerst zu.' WHERE id = 5875;</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>5966</v>
+        <v>5881</v>
       </c>
       <c r="B84" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="C84">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="D84" t="s">
-        <v>114</v>
+        <v>466</v>
       </c>
       <c r="E84">
         <v>14</v>
@@ -14173,169 +14213,172 @@
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Heilt 1 LP pro Benutzung, kann 3x heilen.' WHERE id = 5966;</v>
+        <f>CONCATENATE("UPDATE ",H84," SET description = '",D84,"' WHERE id = ",A84,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Zweihändige Axt, Paraderune (-1 auf Attacken von Gegner), Schadensrune (Schaden: W6)' WHERE id = 5881;</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>6013</v>
+        <v>5884</v>
       </c>
       <c r="B85" t="s">
-        <v>171</v>
+        <v>52</v>
       </c>
       <c r="C85">
-        <v>55</v>
-      </c>
-      <c r="D85" t="s">
-        <v>471</v>
+        <v>65</v>
       </c>
       <c r="E85">
         <v>14</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85">
         <v>1</v>
       </c>
       <c r="H85" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Steinrune (+1 auf RW), Eisenrune (+1 auf W)' WHERE id = 6013;</v>
+        <f>CONCATENATE("UPDATE ",H85," SET description = '",D85,"' WHERE id = ",A85,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5884;</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>6029</v>
+        <v>5892</v>
       </c>
       <c r="B86" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="C86">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="D86" t="s">
-        <v>475</v>
+        <v>377</v>
       </c>
       <c r="E86">
         <v>14</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86">
         <v>1</v>
       </c>
       <c r="H86" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = 'Meisterune der Furcht (1x pro Spiel Einheit unbeweglich, wenn Moraltest mißlingt)' WHERE id = 6029;</v>
+        <f>CONCATENATE("UPDATE ",H86," SET description = '",D86,"' WHERE id = ",A86,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Schadenswurf ist immer 2+. Nur magische Rüstungen mit -3 auf RW. Jede Verletztung kostet W3 LP. Drachen und Dämonen verlieren W6 LP.' WHERE id = 5892;</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>6031</v>
+        <v>5903</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="C87">
-        <v>75</v>
+        <v>165</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>467</v>
       </c>
       <c r="E87">
         <v>14</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87">
         <v>1</v>
       </c>
       <c r="H87" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '' WHERE id = 6031;</v>
+        <f>CONCATENATE("UPDATE ",H87," SET description = '",D87,"' WHERE id = ",A87,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+1 auf Attacken, Stärke: 10, automatischer Schaden wenn Gegner durch Feuer verwundbar, Schaden: W6' WHERE id = 5903;</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>6049</v>
+        <v>5905</v>
       </c>
       <c r="B88" t="s">
-        <v>163</v>
+        <v>67</v>
       </c>
       <c r="C88">
-        <v>25</v>
+        <v>170</v>
+      </c>
+      <c r="D88" t="s">
+        <v>468</v>
       </c>
       <c r="E88">
         <v>14</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88">
         <v>1</v>
       </c>
       <c r="H88" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '' WHERE id = 6049;</v>
+        <f>CONCATENATE("UPDATE ",H88," SET description = '",D88,"' WHERE id = ",A88,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Meisterrune des Todes (Jede Verletzung tötet), Kampfgeschickrune (+1 auf KG), Kraftrune (Stärke x2 gegen Gegner mit mehr Widerstand)' WHERE id = 5905;</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>5954</v>
+        <v>5917</v>
       </c>
       <c r="B89" t="s">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="C89">
-        <v>125</v>
+        <v>75</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="E89">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89">
         <v>1</v>
       </c>
       <c r="H89" t="s">
-        <v>106</v>
+        <v>476</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Misc SET description = '' WHERE id = 5954;</v>
+        <f>CONCATENATE("UPDATE ",H89," SET description = '",D89,"' WHERE id = ",A89,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+2 auf Stärke, nicht zuletzt zuschlagen, 2 Würfel pro Treffer- und Schadenswurf besseres Ergebnis zählt, 2 Würfel für Rettungswurf der Gegner schlechteres Ergebnis zählt' WHERE id = 5917;</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>5908</v>
+        <v>5938</v>
       </c>
       <c r="B90" t="s">
-        <v>190</v>
+        <v>95</v>
       </c>
       <c r="C90">
-        <v>50</v>
-      </c>
-      <c r="D90" t="s">
-        <v>440</v>
+        <v>110</v>
       </c>
       <c r="E90">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -14344,58 +14387,58 @@
         <v>1</v>
       </c>
       <c r="H90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Ranged_Weapon SET description = 'Reichweite: 36", Stärke: 6 -1 pro Glied, Paniktest für Dunkelelfen' WHERE id = 5908;</v>
+        <f>CONCATENATE("UPDATE ",H90," SET description = '",D90,"' WHERE id = ",A90,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '' WHERE id = 5938;</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>5971</v>
+        <v>5973</v>
       </c>
       <c r="B91" t="s">
-        <v>189</v>
+        <v>54</v>
       </c>
       <c r="C91">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D91" t="s">
-        <v>460</v>
+        <v>376</v>
       </c>
       <c r="E91">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91">
         <v>1</v>
       </c>
       <c r="H91" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Ranged_Weapon SET description = 'Reichweite: 36", Stärke: 5, Dreifachschuß' WHERE id = 5971;</v>
+        <f>CONCATENATE("UPDATE ",H91," SET description = '",D91,"' WHERE id = ",A91,";")</f>
+        <v>UPDATE Melee_Weapon SET description = '+2 auf Attacken' WHERE id = 5973;</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>5776</v>
+        <v>6050</v>
       </c>
       <c r="B92" t="s">
-        <v>409</v>
+        <v>77</v>
       </c>
       <c r="C92">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D92" t="s">
-        <v>408</v>
+        <v>469</v>
       </c>
       <c r="E92">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -14404,28 +14447,25 @@
         <v>1</v>
       </c>
       <c r="H92" t="s">
-        <v>194</v>
+        <v>476</v>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Shield SET description = 'Bei eigenem RW, erleidet der Gegner einen Treffer der Stärke 4.' WHERE id = 5776;</v>
+        <f>CONCATENATE("UPDATE ",H92," SET description = '",D92,"' WHERE id = ",A92,";")</f>
+        <v>UPDATE Melee_Weapon SET description = 'Immun gegen Feuer und Hitze, 1x pro Spiel automatischer Magie Bann, normale Bewegung durch schwieriges Gelände' WHERE id = 6050;</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>5840</v>
+        <v>5882</v>
       </c>
       <c r="B93" t="s">
-        <v>417</v>
+        <v>119</v>
       </c>
       <c r="C93">
-        <v>10</v>
-      </c>
-      <c r="D93" t="s">
-        <v>416</v>
+        <v>50</v>
       </c>
       <c r="E93">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F93">
         <v>0</v>
@@ -14434,28 +14474,28 @@
         <v>1</v>
       </c>
       <c r="H93" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Standard SET description = 'Ignoriert die Auswirkung von Blödheit. Nur für Echsenreiter.' WHERE id = 5840;</v>
+        <f>CONCATENATE("UPDATE ",H93," SET description = '",D93,"' WHERE id = ",A93,";")</f>
+        <v>UPDATE Misc SET description = '' WHERE id = 5882;</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>5842</v>
+        <v>5889</v>
       </c>
       <c r="B94" t="s">
-        <v>200</v>
+        <v>132</v>
       </c>
       <c r="C94">
         <v>25</v>
       </c>
       <c r="D94" t="s">
-        <v>201</v>
+        <v>474</v>
       </c>
       <c r="E94">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -14464,28 +14504,28 @@
         <v>1</v>
       </c>
       <c r="H94" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Standard SET description = 'Gegner muss Moraltest bestehen um Jungferngarde anzugreifen.' WHERE id = 5842;</v>
+        <f>CONCATENATE("UPDATE ",H94," SET description = '",D94,"' WHERE id = ",A94,";")</f>
+        <v>UPDATE Misc SET description = 'Erzeugt Flammenwall in 6" Entfernung' WHERE id = 5889;</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>5835</v>
+        <v>5966</v>
       </c>
       <c r="B95" t="s">
-        <v>393</v>
+        <v>113</v>
       </c>
       <c r="C95">
         <v>25</v>
       </c>
       <c r="D95" t="s">
-        <v>392</v>
+        <v>114</v>
       </c>
       <c r="E95">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -14494,28 +14534,28 @@
         <v>1</v>
       </c>
       <c r="H95" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Standard SET description = 'Einheit erhält +1 auf Stärke in der ersten Kampfrunde.' WHERE id = 5835;</v>
+        <f>CONCATENATE("UPDATE ",H95," SET description = '",D95,"' WHERE id = ",A95,";")</f>
+        <v>UPDATE Misc SET description = 'Heilt 1 LP pro Benutzung, kann 3x heilen.' WHERE id = 5966;</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>5836</v>
+        <v>6013</v>
       </c>
       <c r="B96" t="s">
-        <v>391</v>
+        <v>171</v>
       </c>
       <c r="C96">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D96" t="s">
-        <v>390</v>
+        <v>471</v>
       </c>
       <c r="E96">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F96">
         <v>0</v>
@@ -14524,28 +14564,28 @@
         <v>1</v>
       </c>
       <c r="H96" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Standard SET description = 'Jeden verpatzten Stänkerei-Test wiederholen.' WHERE id = 5836;</v>
+        <f>CONCATENATE("UPDATE ",H96," SET description = '",D96,"' WHERE id = ",A96,";")</f>
+        <v>UPDATE Misc SET description = 'Steinrune (+1 auf RW), Eisenrune (+1 auf W)' WHERE id = 6013;</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>5837</v>
+        <v>6029</v>
       </c>
       <c r="B97" t="s">
-        <v>389</v>
+        <v>120</v>
       </c>
       <c r="C97">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D97" t="s">
-        <v>388</v>
+        <v>475</v>
       </c>
       <c r="E97">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F97">
         <v>0</v>
@@ -14554,28 +14594,25 @@
         <v>1</v>
       </c>
       <c r="H97" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Standard SET description = 'Magie Bann bei 4+. Zauberer in Base-to-Base-Kontakt platzt der Kopf.' WHERE id = 5837;</v>
+        <f>CONCATENATE("UPDATE ",H97," SET description = '",D97,"' WHERE id = ",A97,";")</f>
+        <v>UPDATE Misc SET description = 'Meisterune der Furcht (1x pro Spiel Einheit unbeweglich, wenn Moraltest mißlingt)' WHERE id = 6029;</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>5838</v>
+        <v>6031</v>
       </c>
       <c r="B98" t="s">
-        <v>387</v>
+        <v>122</v>
       </c>
       <c r="C98">
-        <v>35</v>
-      </c>
-      <c r="D98" t="s">
-        <v>386</v>
+        <v>75</v>
       </c>
       <c r="E98">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -14584,41 +14621,41 @@
         <v>1</v>
       </c>
       <c r="H98" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="I98" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Standard SET description = '-1 auf Beschuß, Nachtgoblins attackieren immer zuerst' WHERE id = 5838;</v>
+        <f>CONCATENATE("UPDATE ",H98," SET description = '",D98,"' WHERE id = ",A98,";")</f>
+        <v>UPDATE Misc SET description = '' WHERE id = 6031;</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>5839</v>
+        <v>6049</v>
       </c>
       <c r="B99" t="s">
-        <v>385</v>
+        <v>163</v>
       </c>
       <c r="C99">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D99" t="s">
-        <v>384</v>
+        <v>479</v>
       </c>
       <c r="E99">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99">
         <v>1</v>
       </c>
       <c r="H99" t="s">
-        <v>199</v>
+        <v>106</v>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="1"/>
-        <v>UPDATE Standard SET description = 'Verdoppelt Attacken in der ersten Kampfrunde. Nur für Waldgoblins.' WHERE id = 5839;</v>
+        <f>CONCATENATE("UPDATE ",H99," SET description = '",D99,"' WHERE id = ",A99,";")</f>
+        <v>UPDATE Misc SET description = 'Einheiten in 12" Umkreis sammeln sich automatisch' WHERE id = 6049;</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -14644,13 +14681,14 @@
         <v>199</v>
       </c>
       <c r="I100" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("UPDATE ",H100," SET description = '",D100,"' WHERE id = ",A100,";")</f>
         <v>UPDATE Standard SET description = '' WHERE id = 5871;</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H100">
-    <sortCondition ref="H2:H100"/>
+  <autoFilter ref="A1:I100" xr:uid="{1508439D-2206-4762-B104-9E5E275BF891}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I100">
+    <sortCondition ref="E2:E100"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>